<commit_message>
Agregamos gráficos a BNLJ
TODOs
Terminar conclusiones
Revisar la sección BNLJ
</commit_message>
<xml_diff>
--- a/tp2/resultados/bnlj_r_mayor_a_s.xlsx
+++ b/tp2/resultados/bnlj_r_mayor_a_s.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="360" yWindow="105" windowWidth="19920" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="5" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="268">
   <si>
     <t>LRUReplacementStrategy</t>
   </si>
@@ -764,6 +765,63 @@
   </si>
   <si>
     <t>&gt;&gt; H : {[[S, 0]][[S, 1]][[S, 2]][[S, 3]][[S, 4]][[S, 5]][[S, 6]][[S, 7]][[S, 8]][[S, 9]][[R, 30]][[R, 31]][[R, 32]][[R, 33]][[R, 34]][[S, 15]][[S, 16]][[S, 17]][[S, 18]][[S, 19]][[R, 45]][[R, 46]][[R, 47]][[R, 48]][[R, 49]][[R, 35]][[R, 36]][[R, 37]][[R, 38]][[R, 39]][[R, 40]][[R, 41]][[R, 42]][[R, 43]][[R, 44]][[S, 10]][[S, 11]][[S, 12]][[S, 13]][[S, 14]]}</t>
+  </si>
+  <si>
+    <t>R20-S50-b1-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b2-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b3-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b4-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b5-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b6-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b7-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b8-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b9-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b10-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b11-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b12-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b13-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b14-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b15-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b16-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b17-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b18-BuffSize40</t>
+  </si>
+  <si>
+    <t>R20-S50-b19-BuffSize40</t>
   </si>
 </sst>
 </file>
@@ -825,6 +883,278 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-AR"/>
   <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja5!$D$20:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MRU</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja5!$D$39:$D$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja5!$D$1:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="68926848"/>
+        <c:axId val="69189632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="68926848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69189632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69189632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="68926848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
@@ -1049,13 +1379,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="59834368"/>
-        <c:axId val="70913408"/>
+        <c:axId val="70537600"/>
+        <c:axId val="70539520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59834368"/>
+        <c:axId val="70537600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,14 +1409,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70913408"/>
+        <c:crossAx val="70539520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70913408"/>
+        <c:axId val="70539520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1442,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59834368"/>
+        <c:crossAx val="70537600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,13 +1455,48 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1454,7 +1818,827 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>252</v>
+      </c>
+      <c r="B23">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>254</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>255</v>
+      </c>
+      <c r="B26">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>256</v>
+      </c>
+      <c r="B27">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>257</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>259</v>
+      </c>
+      <c r="B30">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>261</v>
+      </c>
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B33">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>263</v>
+      </c>
+      <c r="B34">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>264</v>
+      </c>
+      <c r="B35">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>265</v>
+      </c>
+      <c r="B36">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>266</v>
+      </c>
+      <c r="B37">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>267</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>251</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>255</v>
+      </c>
+      <c r="B45">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>256</v>
+      </c>
+      <c r="B46">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>257</v>
+      </c>
+      <c r="B47">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>258</v>
+      </c>
+      <c r="B48">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>259</v>
+      </c>
+      <c r="B49">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>260</v>
+      </c>
+      <c r="B50">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>262</v>
+      </c>
+      <c r="B52">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>263</v>
+      </c>
+      <c r="B53">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>264</v>
+      </c>
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>265</v>
+      </c>
+      <c r="B55">
+        <v>40</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>266</v>
+      </c>
+      <c r="B56">
+        <v>40</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>267</v>
+      </c>
+      <c r="B57">
+        <v>40</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0.17</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:D57">
+    <sortCondition ref="C1:C57"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -2270,7 +3454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D131"/>
   <sheetViews>
@@ -2950,7 +4134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D131"/>
   <sheetViews>
@@ -3629,7 +4813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
correcciones en el POM para que se genere bien el jar  comentarios en DemoStrategy y correccion de la ruta de los traces
</commit_message>
<xml_diff>
--- a/tp2/resultados/bnlj_r_mayor_a_s.xlsx
+++ b/tp2/resultados/bnlj_r_mayor_a_s.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="19920" windowHeight="8010"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="19920" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja5" sheetId="5" r:id="rId1"/>
@@ -1106,6 +1106,7 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls/>
         <c:marker val="1"/>
         <c:axId val="68926848"/>
         <c:axId val="69189632"/>
@@ -1116,6 +1117,25 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Bloques para R</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="69189632"/>
         <c:crosses val="autoZero"/>
@@ -1130,6 +1150,24 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>HitRate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="68926848"/>
@@ -1466,13 +1504,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>539863</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
+      <xdr:colOff>730363</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -1818,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="A3" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2638,7 +2676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -3458,8 +3496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView topLeftCell="D108" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64:R131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>